<commit_message>
Final version of working code
</commit_message>
<xml_diff>
--- a/initial_params.xlsx
+++ b/initial_params.xlsx
@@ -475,7 +475,7 @@
         <v>0.01</v>
       </c>
       <c r="H2">
-        <v>-0.5382516940701341</v>
+        <v>-1.98908430042096</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -507,7 +507,7 @@
         <v>0.01</v>
       </c>
       <c r="H3">
-        <v>-0.3122190014324168</v>
+        <v>-1.448638050480701</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -584,7 +584,7 @@
         <v>0.01</v>
       </c>
       <c r="H2">
-        <v>-2.432000621081636</v>
+        <v>-2.833048256440481</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>0.01</v>
       </c>
       <c r="H3">
-        <v>-2.338056636100122</v>
+        <v>-2.395648834918044</v>
       </c>
       <c r="I3">
         <v>1</v>

</xml_diff>